<commit_message>
better clean string routine, remove white spaces
</commit_message>
<xml_diff>
--- a/data/bornpowerindex.xlsx
+++ b/data/bornpowerindex.xlsx
@@ -37,13 +37,13 @@
     <t>APPRENTICE-NEWPORT NEWS</t>
   </si>
   <si>
-    <t>ATLANTIS  -  FLA</t>
+    <t>ATLANTIS - FLA</t>
   </si>
   <si>
     <t>FORT LAUDERDALE</t>
   </si>
   <si>
-    <t>LINCOLN -  CALIFONIA</t>
+    <t>LINCOLN - CALIFONIA</t>
   </si>
   <si>
     <t>NORTH AMERICAN - TEXAS</t>
@@ -79,7 +79,7 @@
     <t>BETHEL-TN.</t>
   </si>
   <si>
-    <t>BLUEFIELD  -  VA</t>
+    <t>BLUEFIELD - VA</t>
   </si>
   <si>
     <t>BRIAR CLIFF</t>
@@ -184,7 +184,7 @@
     <t>LOUISIANA CHRISTIAN</t>
   </si>
   <si>
-    <t>MADONNA  - MICHIGAN</t>
+    <t>MADONNA - MICHIGAN</t>
   </si>
   <si>
     <t>MARIAN - INDIANA</t>
@@ -196,7 +196,7 @@
     <t>McPHERSON</t>
   </si>
   <si>
-    <t>MID-AMERICA  NAZARENE</t>
+    <t>MID-AMERICA NAZARENE</t>
   </si>
   <si>
     <t>MIDLAND - NE</t>
@@ -220,7 +220,7 @@
     <t>MORNINGSIDE</t>
   </si>
   <si>
-    <t xml:space="preserve">MT.  MARTY    S.D. </t>
+    <t xml:space="preserve">MT. MARTY S.D. </t>
   </si>
   <si>
     <t>NORTHWESTERN-IOWA</t>
@@ -229,7 +229,7 @@
     <t>OLIVET NAZARENE</t>
   </si>
   <si>
-    <t>OTTAWA  (AZ)</t>
+    <t>OTTAWA (AZ)</t>
   </si>
   <si>
     <t>OTTAWA-KANSAS</t>
@@ -304,7 +304,7 @@
     <t>TEXAS WESLEYAN</t>
   </si>
   <si>
-    <t>THOMAS  -  GA</t>
+    <t>THOMAS - GA</t>
   </si>
   <si>
     <t>UNION-KY.</t>
@@ -334,7 +334,7 @@
     <t>ABILENE CHRISTIAN</t>
   </si>
   <si>
-    <t>ALABAMA  A&amp;M</t>
+    <t>ALABAMA A&amp;M</t>
   </si>
   <si>
     <t>ALABAMA STATE</t>
@@ -409,7 +409,7 @@
     <t>DELAWARE</t>
   </si>
   <si>
-    <t>DELAWARE  STATE</t>
+    <t>DELAWARE STATE</t>
   </si>
   <si>
     <t>DRAKE</t>
@@ -433,7 +433,7 @@
     <t>ELON</t>
   </si>
   <si>
-    <t>FLORIDA  A&amp;M</t>
+    <t>FLORIDA A&amp;M</t>
   </si>
   <si>
     <t>FORDHAM</t>
@@ -553,7 +553,7 @@
     <t>NORTH ALABAMA</t>
   </si>
   <si>
-    <t>NORTH CAROLINA  A&amp;T</t>
+    <t>NORTH CAROLINA A&amp;T</t>
   </si>
   <si>
     <t>NORTH CAROLINA CENTRAL</t>
@@ -628,7 +628,7 @@
     <t>SOUTH DAKOTA STATE</t>
   </si>
   <si>
-    <t>SOUTH EASTERN  MISSOURI</t>
+    <t>SOUTH EASTERN MISSOURI</t>
   </si>
   <si>
     <t>SOUTHERN ILLINOIS</t>
@@ -724,7 +724,7 @@
     <t>ALDERSON-BROADDUS</t>
   </si>
   <si>
-    <t>ALLEN  (SC)</t>
+    <t>ALLEN (SC)</t>
   </si>
   <si>
     <t>AMERICAN INTERNATIONAL</t>
@@ -994,7 +994,7 @@
     <t>MOREHOUSE COLLEGE</t>
   </si>
   <si>
-    <t>NEBRASKA -  KEARNEY</t>
+    <t>NEBRASKA - KEARNEY</t>
   </si>
   <si>
     <t>NEWBERRY</t>
@@ -1006,7 +1006,7 @@
     <t>NEW MEXICO HIGHLANDS</t>
   </si>
   <si>
-    <t>NO'EASTERN   OKLA ST.</t>
+    <t>NOEASTERN OKLA ST.</t>
   </si>
   <si>
     <t>NORTHERN MICHIGAN</t>
@@ -1084,7 +1084,7 @@
     <t>SO. EAST. OKLAHOMA ST.</t>
   </si>
   <si>
-    <t>SOUTH DAKOTA  TECH</t>
+    <t>SOUTH DAKOTA TECH</t>
   </si>
   <si>
     <t>SOUTHERN ARKANSAS</t>
@@ -1195,7 +1195,7 @@
     <t>WEST VIRGINIA WESLEYAN</t>
   </si>
   <si>
-    <t>WHEELING  UNIVERSITY</t>
+    <t>WHEELING UNIVERSITY</t>
   </si>
   <si>
     <t>WILLIAM JEWELL</t>
@@ -1276,7 +1276,7 @@
     <t>BERRY</t>
   </si>
   <si>
-    <t>BETHANY  -  WV</t>
+    <t>BETHANY - WV</t>
   </si>
   <si>
     <t>BETHEL-MINNESOTA</t>
@@ -1408,7 +1408,7 @@
     <t>DUBUQUE</t>
   </si>
   <si>
-    <t>EASTERN  PA</t>
+    <t>EASTERN PA</t>
   </si>
   <si>
     <t>EAST TEXAS BAPTIST</t>
@@ -1546,7 +1546,7 @@
     <t>KEYSTONE</t>
   </si>
   <si>
-    <t>KING'S COLLEGE</t>
+    <t>KINGS COLLEGE</t>
   </si>
   <si>
     <t>KNOX</t>
@@ -1663,7 +1663,7 @@
     <t>MUSKINGUM</t>
   </si>
   <si>
-    <t>NEBRASKA  WESLEYAN</t>
+    <t>NEBRASKA WESLEYAN</t>
   </si>
   <si>
     <t>NEW JERSEY</t>
@@ -1819,7 +1819,7 @@
     <t xml:space="preserve">UNION COLLEGE-NY </t>
   </si>
   <si>
-    <t>U  O F  NEW ENGLAND</t>
+    <t>U O F NEW ENGLAND</t>
   </si>
   <si>
     <t>URSINUS COLLEGE</t>
@@ -2047,7 +2047,7 @@
     <t>GEORGIA TECH</t>
   </si>
   <si>
-    <t>HAWAI'I</t>
+    <t>HAWAII</t>
   </si>
   <si>
     <t>HOUSTON</t>
@@ -2161,13 +2161,13 @@
     <t>NO. CAROLINA STATE</t>
   </si>
   <si>
-    <t>NORTH  CAROLINA</t>
-  </si>
-  <si>
-    <t>NORTHERN  ILLINOIS</t>
-  </si>
-  <si>
-    <t>NORTH  TEXAS</t>
+    <t>NORTH CAROLINA</t>
+  </si>
+  <si>
+    <t>NORTHERN ILLINOIS</t>
+  </si>
+  <si>
+    <t>NORTH TEXAS</t>
   </si>
   <si>
     <t>NORTHWESTERN</t>
@@ -2233,7 +2233,7 @@
     <t>SOUTHERN METHODIST</t>
   </si>
   <si>
-    <t>SOUTHERN  MISSISSIPPI</t>
+    <t>SOUTHERN MISSISSIPPI</t>
   </si>
   <si>
     <t>SOUTH FLORIDA</t>
@@ -2266,7 +2266,7 @@
     <t>TEXAS-SAN ANTONIO</t>
   </si>
   <si>
-    <t>TEXAS  STATE-SAN MARCOS</t>
+    <t>TEXAS STATE-SAN MARCOS</t>
   </si>
   <si>
     <t>TEXAS TECH</t>
@@ -2320,7 +2320,7 @@
     <t>WESTERN MICHIGAN</t>
   </si>
   <si>
-    <t>WEST  VIRGINIA</t>
+    <t>WEST VIRGINIA</t>
   </si>
   <si>
     <t>WISCONSIN</t>
@@ -2620,90 +2620,90 @@
     <t>USM</t>
   </si>
   <si>
+    <t>EIU</t>
+  </si>
+  <si>
+    <t>USF</t>
+  </si>
+  <si>
+    <t>STAN</t>
+  </si>
+  <si>
+    <t>SYR</t>
+  </si>
+  <si>
+    <t>TEM</t>
+  </si>
+  <si>
+    <t>TENN</t>
+  </si>
+  <si>
+    <t>TEX</t>
+  </si>
+  <si>
+    <t>TA&amp;M</t>
+  </si>
+  <si>
+    <t>ACU</t>
+  </si>
+  <si>
+    <t>TXST</t>
+  </si>
+  <si>
+    <t>EWU</t>
+  </si>
+  <si>
+    <t>WCU</t>
+  </si>
+  <si>
+    <t>TTU</t>
+  </si>
+  <si>
+    <t>COLG</t>
+  </si>
+  <si>
+    <t>MUR</t>
+  </si>
+  <si>
+    <t>TULN</t>
+  </si>
+  <si>
+    <t>TLSA</t>
+  </si>
+  <si>
+    <t>BUCK</t>
+  </si>
+  <si>
+    <t>CLT</t>
+  </si>
+  <si>
+    <t>USU</t>
+  </si>
+  <si>
+    <t>VAN</t>
+  </si>
+  <si>
+    <t>UVA</t>
+  </si>
+  <si>
+    <t>VT</t>
+  </si>
+  <si>
+    <t>WAKE</t>
+  </si>
+  <si>
+    <t>WSU</t>
+  </si>
+  <si>
+    <t>JKST</t>
+  </si>
+  <si>
+    <t>WKU</t>
+  </si>
+  <si>
     <t>WIU</t>
   </si>
   <si>
-    <t>USF</t>
-  </si>
-  <si>
-    <t>STAN</t>
-  </si>
-  <si>
-    <t>SYR</t>
-  </si>
-  <si>
-    <t>TEM</t>
-  </si>
-  <si>
-    <t>TENN</t>
-  </si>
-  <si>
-    <t>TEX</t>
-  </si>
-  <si>
-    <t>TA&amp;M</t>
-  </si>
-  <si>
-    <t>HCU</t>
-  </si>
-  <si>
-    <t>TXST</t>
-  </si>
-  <si>
-    <t>EWU</t>
-  </si>
-  <si>
-    <t>WCU</t>
-  </si>
-  <si>
-    <t>TTU</t>
-  </si>
-  <si>
-    <t>COLG</t>
-  </si>
-  <si>
-    <t>MUR</t>
-  </si>
-  <si>
-    <t>TULN</t>
-  </si>
-  <si>
-    <t>TLSA</t>
-  </si>
-  <si>
-    <t>BUCK</t>
-  </si>
-  <si>
-    <t>CLT</t>
-  </si>
-  <si>
-    <t>USU</t>
-  </si>
-  <si>
-    <t>VAN</t>
-  </si>
-  <si>
-    <t>UVA</t>
-  </si>
-  <si>
-    <t>VT</t>
-  </si>
-  <si>
-    <t>WAKE</t>
-  </si>
-  <si>
-    <t>WSU</t>
-  </si>
-  <si>
-    <t>YSU</t>
-  </si>
-  <si>
-    <t>WKU</t>
-  </si>
-  <si>
-    <t>NWST</t>
-  </si>
-  <si>
     <t>WVU</t>
   </si>
   <si>
@@ -2728,7 +2728,7 @@
     <t>DIVISION 3</t>
   </si>
   <si>
-    <t>DIVISION 1  FBS</t>
+    <t>DIVISION 1 FBS</t>
   </si>
   <si>
     <t>5.7</t>
@@ -18298,7 +18298,7 @@
         <v>1417</v>
       </c>
       <c r="F673">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="674" spans="1:6">
@@ -19058,7 +19058,7 @@
         <v>1450</v>
       </c>
       <c r="F711">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="712" spans="1:6">
@@ -19078,7 +19078,7 @@
         <v>1085</v>
       </c>
       <c r="F712">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="713" spans="1:6">
@@ -19098,7 +19098,7 @@
         <v>1451</v>
       </c>
       <c r="F713">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="714" spans="1:6">
@@ -19538,7 +19538,7 @@
         <v>1467</v>
       </c>
       <c r="F735">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="736" spans="1:6">
@@ -19758,7 +19758,7 @@
         <v>1476</v>
       </c>
       <c r="F746">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="747" spans="1:6">
@@ -20098,7 +20098,7 @@
         <v>1070</v>
       </c>
       <c r="F763">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="764" spans="1:6">
@@ -20118,7 +20118,7 @@
         <v>1485</v>
       </c>
       <c r="F764">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="765" spans="1:6">

</xml_diff>